<commit_message>
Form changes, Logging changes and new test data overview
</commit_message>
<xml_diff>
--- a/TestData/TestdataOverview.xlsx
+++ b/TestData/TestdataOverview.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biermapa\source\repos\cosurv-smics\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="23715" windowHeight="8265" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="23715" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Movement" sheetId="1" r:id="rId1"/>
@@ -23,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="384">
   <si>
     <t>Impfstoff</t>
   </si>
@@ -1091,12 +1086,96 @@
   </si>
   <si>
     <t>2021-01-09T09:00:00</t>
+  </si>
+  <si>
+    <t>2021-01-03T15:00:00</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>LA Klin.Auftrag</t>
+  </si>
+  <si>
+    <t>Herzchirurgie</t>
+  </si>
+  <si>
+    <t>3600</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>0300</t>
+  </si>
+  <si>
+    <t>0500</t>
+  </si>
+  <si>
+    <t>2021-01-03T19:40:00</t>
+  </si>
+  <si>
+    <t>2021-01-04T10:40:00</t>
+  </si>
+  <si>
+    <t>2021-01-06T15:00:00</t>
+  </si>
+  <si>
+    <t>2021-01-06T17:34:00</t>
+  </si>
+  <si>
+    <t>Pneumologie</t>
+  </si>
+  <si>
+    <t>0800</t>
+  </si>
+  <si>
+    <t>2021-01-07T12:34:00</t>
+  </si>
+  <si>
+    <t>Lungen- und Bronchialheilkunde</t>
+  </si>
+  <si>
+    <t>1400</t>
+  </si>
+  <si>
+    <t>2021-01-08T15:25:00</t>
+  </si>
+  <si>
+    <t>2021-01-04T15:46:00</t>
+  </si>
+  <si>
+    <t>Neurologie</t>
+  </si>
+  <si>
+    <t>2800</t>
+  </si>
+  <si>
+    <t>2021-01-05T09:46:00</t>
+  </si>
+  <si>
+    <t>Strahlenheilkunde</t>
+  </si>
+  <si>
+    <t>3300</t>
+  </si>
+  <si>
+    <t>2021-01-06T10:46:00</t>
+  </si>
+  <si>
+    <t>2021-01-06T11:36:00</t>
+  </si>
+  <si>
+    <t>2021-01-02T09:45:00</t>
+  </si>
+  <si>
+    <t>2021-01-03T13:48:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1254,7 +1333,13 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1281,9 +1366,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1328,12 +1410,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="B5:J58" totalsRowShown="0" headerRowDxfId="12">
-  <autoFilter ref="B5:J58"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="B5:K73" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="B5:K73"/>
+  <tableColumns count="10">
     <tableColumn id="1" name="//"/>
     <tableColumn id="2" name="ehr_id"/>
-    <tableColumn id="3" name="Station" dataDxfId="11"/>
+    <tableColumn id="3" name="Station" dataDxfId="1"/>
+    <tableColumn id="10" name="code_string" dataDxfId="0"/>
     <tableColumn id="4" name="Fachabteilungsschlüssel"/>
     <tableColumn id="5" name="Beginn"/>
     <tableColumn id="6" name="Ende"/>
@@ -1372,8 +1455,8 @@
   <tableColumns count="14">
     <tableColumn id="1" name="//"/>
     <tableColumn id="2" name="ehr_id"/>
-    <tableColumn id="3" name="Bericht ID" dataDxfId="10"/>
-    <tableColumn id="4" name="Fall-Kennung" dataDxfId="9"/>
+    <tableColumn id="3" name="Bericht ID" dataDxfId="12"/>
+    <tableColumn id="4" name="Fall-Kennung" dataDxfId="11"/>
     <tableColumn id="5" name="Laborprobenidentifikator"/>
     <tableColumn id="6" name="Zeitpunkt Probeentnahme"/>
     <tableColumn id="7" name="Zeitpunkt des Probeneingangs"/>
@@ -1390,17 +1473,17 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B4:I19" totalsRowShown="0" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B4:I19" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="B4:I19"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="//" dataDxfId="7"/>
-    <tableColumn id="2" name="ehr_id" dataDxfId="6"/>
-    <tableColumn id="3" name="Impfstoff" dataDxfId="5"/>
-    <tableColumn id="4" name="Dosierungsreihenfolge" dataDxfId="4"/>
-    <tableColumn id="5" name="Dosiermenge" dataDxfId="3"/>
-    <tableColumn id="6" name="Impfung gegen" dataDxfId="2"/>
-    <tableColumn id="7" name="Abwesenheit" dataDxfId="1"/>
-    <tableColumn id="8" name="start_time" dataDxfId="0"/>
+    <tableColumn id="1" name="//" dataDxfId="9"/>
+    <tableColumn id="2" name="ehr_id" dataDxfId="8"/>
+    <tableColumn id="3" name="Impfstoff" dataDxfId="7"/>
+    <tableColumn id="4" name="Dosierungsreihenfolge" dataDxfId="6"/>
+    <tableColumn id="5" name="Dosiermenge" dataDxfId="5"/>
+    <tableColumn id="6" name="Impfung gegen" dataDxfId="4"/>
+    <tableColumn id="7" name="Abwesenheit" dataDxfId="3"/>
+    <tableColumn id="8" name="start_time" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1424,9 +1507,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1464,9 +1547,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1501,7 +1584,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1536,7 +1619,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1710,29 +1793,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J55"/>
+  <dimension ref="A2:K72"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.85546875" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" customWidth="1"/>
+    <col min="4" max="5" width="19.28515625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>351</v>
       </c>
@@ -1742,26 +1825,27 @@
       <c r="D3" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="J3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1771,23 +1855,23 @@
       <c r="D4" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>60</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>82</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>77</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>29</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1800,716 +1884,803 @@
       <c r="D5" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="G5" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="H5" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="I5" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="J5" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="K5" s="22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
       <c r="D6" s="26"/>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="G6" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="I6" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="J6" s="26" t="s">
         <v>331</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="K6" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
       <c r="D7" s="26"/>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="G7" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="H7" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="I7" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="J7" s="26" t="s">
         <v>332</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="K7" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>3</v>
       </c>
       <c r="D8" s="26"/>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="I8" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="J8" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="K8" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>4</v>
       </c>
       <c r="D9" s="26"/>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="G9" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="H9" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="I9" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="J9" s="26" t="s">
         <v>334</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="K9" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>5</v>
       </c>
       <c r="D10" s="26"/>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F10" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="G10" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="H10" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="I10" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="J10" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="K10" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>5</v>
       </c>
       <c r="D11" s="26"/>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F11" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="G11" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="H11" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="I11" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="J11" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="K11" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="18">
         <v>6</v>
       </c>
       <c r="D12" s="26"/>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F12" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="G12" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="H12" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="I12" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="J12" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="K12" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="18">
         <v>7</v>
       </c>
       <c r="D13" s="26"/>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F13" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="G13" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="H13" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="I13" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="I13" s="26" t="s">
+      <c r="J13" s="26" t="s">
         <v>337</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="K13" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="18">
         <v>8</v>
       </c>
       <c r="D14" s="26"/>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F14" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="G14" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="H14" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="I14" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="J14" s="26" t="s">
         <v>338</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="K14" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="18">
         <v>9</v>
       </c>
       <c r="D15" s="26"/>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F15" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="G15" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="H15" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="I15" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="I15" s="26" t="s">
+      <c r="J15" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="K15" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="18">
         <v>10</v>
       </c>
       <c r="D16" s="26"/>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="F16" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="G16" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="H16" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="I16" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="J16" s="26" t="s">
         <v>340</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="K16" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="18">
         <v>10</v>
       </c>
       <c r="D17" s="26"/>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="F17" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="G17" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="H17" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="H17" s="23" t="s">
+      <c r="I17" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I17" s="26" t="s">
+      <c r="J17" s="26" t="s">
         <v>340</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="K17" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="18">
         <v>11</v>
       </c>
       <c r="D18" s="26"/>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="F18" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="G18" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="H18" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="I18" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I18" s="26" t="s">
+      <c r="J18" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="K18" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="18">
         <v>11</v>
       </c>
       <c r="D19" s="26"/>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="F19" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="G19" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="H19" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="I19" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="J19" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="K19" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="18">
         <v>12</v>
       </c>
       <c r="D20" s="26"/>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="F20" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="G20" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="H20" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="I20" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I20" s="26" t="s">
+      <c r="J20" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="J20" s="23" t="s">
+      <c r="K20" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="18">
         <v>13</v>
       </c>
       <c r="D21" s="26"/>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="F21" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="G21" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="H21" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="I21" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I21" s="26" t="s">
+      <c r="J21" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="J21" s="23" t="s">
+      <c r="K21" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="18">
         <v>13</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>350</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F22" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="G22" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="H22" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="I22" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I22" s="26" t="s">
+      <c r="J22" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="K22" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="18">
         <v>14</v>
       </c>
       <c r="D23" s="26"/>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F23" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="G23" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="H23" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="I23" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="I23" s="26" t="s">
+      <c r="J23" s="26" t="s">
         <v>344</v>
       </c>
-      <c r="J23" s="23" t="s">
+      <c r="K23" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="18">
         <v>15</v>
       </c>
       <c r="D24" s="26"/>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="F24" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="G24" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="H24" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="I24" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I24" s="26" t="s">
+      <c r="J24" s="26" t="s">
         <v>345</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="K24" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="18">
         <v>16</v>
       </c>
       <c r="D25" s="26"/>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="F25" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="G25" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="G25" s="23" t="s">
+      <c r="H25" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="I25" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I25" s="26" t="s">
+      <c r="J25" s="26" t="s">
         <v>346</v>
       </c>
-      <c r="J25" s="23" t="s">
+      <c r="K25" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>17</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F26" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="G26" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="G26" s="23" t="s">
+      <c r="H26" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="H26" s="23" t="s">
+      <c r="I26" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I26" s="26" t="s">
+      <c r="J26" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="J26" s="23" t="s">
+      <c r="K26" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>18</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F27" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="G27" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="G27" s="23" t="s">
+      <c r="H27" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="H27" s="23" t="s">
+      <c r="I27" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I27" s="26" t="s">
+      <c r="J27" s="26" t="s">
         <v>275</v>
       </c>
-      <c r="J27" s="23" t="s">
+      <c r="K27" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>19</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F28" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="G28" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="G28" s="23" t="s">
+      <c r="H28" s="23" t="s">
         <v>282</v>
       </c>
-      <c r="H28" s="23" t="s">
+      <c r="I28" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I28" s="26" t="s">
+      <c r="J28" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="J28" s="23" t="s">
+      <c r="K28" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>19</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F29" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="G29" s="23" t="s">
         <v>282</v>
       </c>
-      <c r="G29" s="23" t="s">
+      <c r="H29" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="H29" s="23" t="s">
+      <c r="I29" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I29" s="26" t="s">
+      <c r="J29" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="J29" s="23" t="s">
+      <c r="K29" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>20</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F30" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="G30" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="H30" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="H30" s="23" t="s">
+      <c r="I30" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I30" s="26" t="s">
+      <c r="J30" s="26" t="s">
         <v>285</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="K30" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>21</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F31" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F31" s="23" t="s">
+      <c r="G31" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="G31" s="23" t="s">
+      <c r="H31" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="H31" s="23" t="s">
+      <c r="I31" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I31" s="26" t="s">
+      <c r="J31" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="J31" s="23" t="s">
+      <c r="K31" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>21</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F32" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F32" s="23" t="s">
+      <c r="G32" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="G32" s="23" t="s">
+      <c r="H32" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="H32" s="23" t="s">
+      <c r="I32" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I32" s="26" t="s">
+      <c r="J32" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="J32" s="23" t="s">
+      <c r="K32" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>21</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="F33" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="F33" s="23" t="s">
+      <c r="G33" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="G33" s="23" t="s">
+      <c r="H33" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="H33" s="23" t="s">
+      <c r="I33" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I33" s="26" t="s">
+      <c r="J33" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="J33" s="23" t="s">
+      <c r="K33" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -2519,23 +2690,26 @@
       <c r="D34" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E34" s="23" t="s">
+      <c r="E34" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F34" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F34" s="23" t="s">
+      <c r="G34" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="H34" s="23" t="s">
+      <c r="I34" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I34" s="26" t="s">
+      <c r="J34" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="J34" s="23" t="s">
+      <c r="K34" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>80</v>
       </c>
@@ -2545,46 +2719,52 @@
       <c r="D35" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F35" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F35" s="23" t="s">
+      <c r="G35" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="H35" s="23" t="s">
+      <c r="I35" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I35" s="26" t="s">
+      <c r="J35" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="J35" s="23" t="s">
+      <c r="K35" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>23</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F36" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F36" s="23" t="s">
+      <c r="G36" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="H36" s="23" t="s">
+      <c r="I36" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I36" s="26" t="s">
+      <c r="J36" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="J36" s="23" t="s">
+      <c r="K36" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -2594,23 +2774,26 @@
       <c r="D37" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F37" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="G37" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="H37" s="23" t="s">
+      <c r="I37" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I37" s="26" t="s">
+      <c r="J37" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="J37" s="23" t="s">
+      <c r="K37" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -2620,23 +2803,26 @@
       <c r="D38" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F38" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F38" s="23" t="s">
+      <c r="G38" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="H38" s="23" t="s">
+      <c r="I38" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I38" s="26" t="s">
+      <c r="J38" s="26" t="s">
         <v>306</v>
       </c>
-      <c r="J38" s="23" t="s">
+      <c r="K38" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -2646,412 +2832,956 @@
       <c r="D39" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="E39" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F39" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="G39" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="H39" s="23" t="s">
+      <c r="I39" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I39" s="26" t="s">
+      <c r="J39" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J39" s="23" t="s">
+      <c r="K39" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>27</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F40" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="G40" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="G40" s="23" t="s">
+      <c r="H40" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="H40" s="23" t="s">
+      <c r="I40" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I40" s="26" t="s">
+      <c r="J40" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J40" s="23" t="s">
+      <c r="K40" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>27</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="E41" s="23" t="s">
+      <c r="E41" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F41" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F41" s="23" t="s">
+      <c r="G41" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="G41" s="23" t="s">
+      <c r="H41" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="H41" s="23" t="s">
+      <c r="I41" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I41" s="26" t="s">
+      <c r="J41" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J41" s="23" t="s">
+      <c r="K41" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>27</v>
       </c>
       <c r="D42" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E42" s="23" t="s">
+      <c r="E42" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F42" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F42" s="23" t="s">
+      <c r="G42" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="H42" s="23" t="s">
+      <c r="I42" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I42" s="26" t="s">
+      <c r="J42" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J42" s="23" t="s">
+      <c r="K42" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>28</v>
       </c>
       <c r="D43" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E43" s="23" t="s">
+      <c r="E43" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F43" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F43" s="23" t="s">
+      <c r="G43" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="H43" s="23" t="s">
+      <c r="I43" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I43" s="26" t="s">
+      <c r="J43" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="J43" s="23" t="s">
+      <c r="K43" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>29</v>
       </c>
       <c r="D44" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E44" s="23" t="s">
+      <c r="E44" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F44" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F44" s="23" t="s">
+      <c r="G44" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="H44" s="23" t="s">
+      <c r="I44" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I44" s="26" t="s">
+      <c r="J44" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="K44" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>30</v>
       </c>
       <c r="D45" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="E45" s="23" t="s">
+      <c r="E45" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F45" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F45" s="23" t="s">
+      <c r="G45" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="G45" s="23" t="s">
+      <c r="H45" s="23" t="s">
         <v>320</v>
       </c>
-      <c r="H45" s="23" t="s">
+      <c r="I45" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I45" s="26" t="s">
+      <c r="J45" s="26" t="s">
         <v>319</v>
       </c>
-      <c r="J45" s="23" t="s">
+      <c r="K45" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>30</v>
       </c>
       <c r="D46" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E46" s="23" t="s">
+      <c r="E46" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F46" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F46" s="23" t="s">
+      <c r="G46" s="23" t="s">
         <v>320</v>
       </c>
-      <c r="H46" s="23" t="s">
+      <c r="I46" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I46" s="26" t="s">
+      <c r="J46" s="26" t="s">
         <v>319</v>
       </c>
-      <c r="J46" s="23" t="s">
+      <c r="K46" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>31</v>
       </c>
       <c r="D47" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="E47" s="23" t="s">
+      <c r="E47" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F47" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="G47" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="G47" s="23" t="s">
+      <c r="H47" s="23" t="s">
         <v>322</v>
       </c>
-      <c r="H47" s="23" t="s">
+      <c r="I47" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I47" s="26" t="s">
+      <c r="J47" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="J47" s="23" t="s">
+      <c r="K47" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>31</v>
       </c>
       <c r="D48" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E48" s="23" t="s">
+      <c r="E48" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F48" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F48" s="23" t="s">
+      <c r="G48" s="23" t="s">
         <v>322</v>
       </c>
-      <c r="H48" s="23" t="s">
+      <c r="I48" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I48" s="26" t="s">
+      <c r="J48" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="J48" s="23" t="s">
+      <c r="K48" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>32</v>
       </c>
       <c r="D49" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="E49" s="23" t="s">
+      <c r="E49" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F49" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F49" s="23" t="s">
+      <c r="G49" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="G49" s="23" t="s">
+      <c r="H49" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="H49" s="23" t="s">
+      <c r="I49" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I49" s="26" t="s">
+      <c r="J49" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="J49" s="23" t="s">
+      <c r="K49" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>32</v>
       </c>
       <c r="D50" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="E50" s="23" t="s">
+      <c r="E50" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F50" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F50" s="23" t="s">
+      <c r="G50" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="G50" s="23" t="s">
+      <c r="H50" s="23" t="s">
         <v>325</v>
       </c>
-      <c r="H50" s="23" t="s">
+      <c r="I50" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I50" s="26" t="s">
+      <c r="J50" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="J50" s="23" t="s">
+      <c r="K50" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>32</v>
       </c>
       <c r="D51" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E51" s="23" t="s">
+      <c r="E51" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F51" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F51" s="23" t="s">
+      <c r="G51" s="23" t="s">
         <v>325</v>
       </c>
-      <c r="G51" s="23" t="s">
+      <c r="H51" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="H51" s="23" t="s">
+      <c r="I51" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I51" s="26" t="s">
+      <c r="J51" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="J51" s="23" t="s">
+      <c r="K51" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>32</v>
       </c>
       <c r="D52" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="E52" s="23" t="s">
+      <c r="E52" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="F52" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="F52" s="23" t="s">
+      <c r="G52" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="H52" s="23" t="s">
+      <c r="I52" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I52" s="26" t="s">
+      <c r="J52" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="J52" s="23" t="s">
+      <c r="K52" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>33</v>
       </c>
       <c r="D53" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E53" s="23" t="s">
+      <c r="E53" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F53" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F53" s="23" t="s">
+      <c r="G53" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="H53" s="23" t="s">
+      <c r="I53" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I53" s="26" t="s">
+      <c r="J53" s="26" t="s">
         <v>328</v>
       </c>
-      <c r="J53" s="23" t="s">
+      <c r="K53" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>34</v>
       </c>
       <c r="D54" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E54" s="23" t="s">
+      <c r="E54" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F54" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F54" s="23" t="s">
+      <c r="G54" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="G54" s="23" t="s">
+      <c r="H54" s="23" t="s">
         <v>330</v>
       </c>
-      <c r="H54" s="23" t="s">
+      <c r="I54" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I54" s="26" t="s">
+      <c r="J54" s="26" t="s">
         <v>329</v>
       </c>
-      <c r="J54" s="23" t="s">
+      <c r="K54" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>34</v>
       </c>
       <c r="D55" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="E55" s="23" t="s">
+      <c r="E55" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="F55" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="F55" s="23" t="s">
+      <c r="G55" s="23" t="s">
         <v>330</v>
       </c>
-      <c r="H55" s="23" t="s">
+      <c r="I55" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I55" s="26" t="s">
+      <c r="J55" s="26" t="s">
         <v>329</v>
       </c>
-      <c r="J55" s="23" t="s">
+      <c r="K55" s="23" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>17</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E56" s="26">
+        <v>2100</v>
+      </c>
+      <c r="F56" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="H56" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="I56" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J56" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="K56" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>17</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="F57" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="G57" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="H57" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="I57" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J57" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="K57" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>17</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E58" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F58" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G58" s="23" t="s">
+        <v>365</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>365</v>
+      </c>
+      <c r="I58" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J58" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="K58" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>20</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E59" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F59" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="I59" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J59" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="K59" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="18">
+        <v>20</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="F60" s="23" t="s">
+        <v>368</v>
+      </c>
+      <c r="G60" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="I60" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J60" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="K60" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="18">
+        <v>20</v>
+      </c>
+      <c r="D61" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="F61" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="H61" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="I61" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J61" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="K61" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="18">
+        <v>20</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E62" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F62" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G62" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="H62" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="I62" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J62" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="K62" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>27</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E63" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="F63" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="G63" s="23" t="s">
+        <v>374</v>
+      </c>
+      <c r="H63" s="23" t="s">
+        <v>374</v>
+      </c>
+      <c r="I63" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J63" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="K63" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="18">
+        <v>27</v>
+      </c>
+      <c r="D64" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E64" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="F64" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="G64" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="H64" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="I64" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J64" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="K64" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" s="18">
+        <v>27</v>
+      </c>
+      <c r="D65" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="F65" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="G65" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="H65" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="I65" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J65" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="K65" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" s="18">
+        <v>27</v>
+      </c>
+      <c r="D66" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E66" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F66" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G66" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="H66" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="I66" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J66" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="K66" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>21</v>
+      </c>
+      <c r="D67" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E67" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F67" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G67" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="H67" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="I67" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J67" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="K67" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="18">
+        <v>21</v>
+      </c>
+      <c r="D68" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E68" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F68" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G68" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="H68" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="I68" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J68" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="K68" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="18">
+        <v>21</v>
+      </c>
+      <c r="D69" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E69" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F69" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G69" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="H69" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="I69" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J69" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="K69" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>30</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E70" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F70" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G70" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="H70" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="I70" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J70" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="K70" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="18">
+        <v>30</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E71" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="F71" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="G71" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="H71" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="I71" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J71" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="K71" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" s="18">
+        <v>30</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E72" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="F72" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G72" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="H72" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="I72" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="J72" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="K72" s="23" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -4017,7 +4747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Test changes and new TestData added (Covid Vaccination)
</commit_message>
<xml_diff>
--- a/TestData/TestdataOverview.xlsx
+++ b/TestData/TestdataOverview.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\B-FAST\GITHub_SmICS\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="23715" windowHeight="8265"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="23715" windowHeight="8265" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Movement" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="393">
   <si>
     <t>Impfstoff</t>
   </si>
@@ -1170,12 +1175,39 @@
   </si>
   <si>
     <t>2021-01-03T13:48:00</t>
+  </si>
+  <si>
+    <t>Vaccine product containing only Severe acute respiratory syndrome coronavirus 2 antigen (medicinal product)</t>
+  </si>
+  <si>
+    <t>Infectious disease (disorder)</t>
+  </si>
+  <si>
+    <t>code_string2</t>
+  </si>
+  <si>
+    <t>2021-01-05T11:30:00Z</t>
+  </si>
+  <si>
+    <t>2021-01-09T10:30:00Z</t>
+  </si>
+  <si>
+    <t>2021-01-07T12:30:00Z</t>
+  </si>
+  <si>
+    <t>Vaccine product containing only Severe acute respiratory syndrome coronavirus 2 messenger ribonucleic acid (medicinal product)</t>
+  </si>
+  <si>
+    <t>2021-01-09T12:30:00Z</t>
+  </si>
+  <si>
+    <t>2021-01-08T16:35:00Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1333,12 +1365,9 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1366,6 +1395,15 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1410,13 +1448,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="B5:K73" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="B5:K73" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="B5:K73"/>
   <tableColumns count="10">
     <tableColumn id="1" name="//"/>
     <tableColumn id="2" name="ehr_id"/>
-    <tableColumn id="3" name="Station" dataDxfId="1"/>
-    <tableColumn id="10" name="code_string" dataDxfId="0"/>
+    <tableColumn id="3" name="Station" dataDxfId="14"/>
+    <tableColumn id="10" name="code_string" dataDxfId="13"/>
     <tableColumn id="4" name="Fachabteilungsschlüssel"/>
     <tableColumn id="5" name="Beginn"/>
     <tableColumn id="6" name="Ende"/>
@@ -1473,14 +1511,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B4:I19" totalsRowShown="0" dataDxfId="10">
-  <autoFilter ref="B4:I19"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B4:K19" totalsRowShown="0" dataDxfId="10">
+  <autoFilter ref="B4:K19"/>
+  <tableColumns count="10">
     <tableColumn id="1" name="//" dataDxfId="9"/>
     <tableColumn id="2" name="ehr_id" dataDxfId="8"/>
+    <tableColumn id="9" name="code_string" dataDxfId="1"/>
     <tableColumn id="3" name="Impfstoff" dataDxfId="7"/>
     <tableColumn id="4" name="Dosierungsreihenfolge" dataDxfId="6"/>
     <tableColumn id="5" name="Dosiermenge" dataDxfId="5"/>
+    <tableColumn id="10" name="code_string2" dataDxfId="0"/>
     <tableColumn id="6" name="Impfung gegen" dataDxfId="4"/>
     <tableColumn id="7" name="Abwesenheit" dataDxfId="3"/>
     <tableColumn id="8" name="start_time" dataDxfId="2"/>
@@ -1507,9 +1547,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1547,9 +1587,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1584,7 +1624,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1619,7 +1659,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1795,7 +1835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
@@ -4747,8 +4787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7359,80 +7399,84 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="4" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="130.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>351</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -7443,142 +7487,314 @@
         <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="23">
+        <v>116077000</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>133</v>
-      </c>
-      <c r="E5" s="25">
-        <v>1</v>
       </c>
       <c r="F5" s="25">
         <v>1</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="25">
+        <v>1</v>
+      </c>
+      <c r="H5" s="23">
+        <v>18624000</v>
+      </c>
+      <c r="I5" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="K5" s="23" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="23">
+        <v>46233009</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>184</v>
-      </c>
-      <c r="E6" s="25">
-        <v>1</v>
       </c>
       <c r="F6" s="25">
         <v>1</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="25">
+        <v>1</v>
+      </c>
+      <c r="H6" s="23">
+        <v>6142004</v>
+      </c>
+      <c r="I6" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="K6" s="23" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>8</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="23">
+        <v>46233009</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>184</v>
-      </c>
-      <c r="E7" s="25">
-        <v>1</v>
       </c>
       <c r="F7" s="25">
         <v>1</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="25">
+        <v>1</v>
+      </c>
+      <c r="H7" s="23">
+        <v>6142004</v>
+      </c>
+      <c r="I7" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="K7" s="23" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>14</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="23">
+        <v>46233009</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>184</v>
-      </c>
-      <c r="E8" s="25">
-        <v>1</v>
       </c>
       <c r="F8" s="25">
         <v>1</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="25">
+        <v>1</v>
+      </c>
+      <c r="H8" s="23">
+        <v>6142004</v>
+      </c>
+      <c r="I8" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="K8" s="23" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>15</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="23">
+        <v>424519000</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>247</v>
-      </c>
-      <c r="E9" s="25">
-        <v>1</v>
       </c>
       <c r="F9" s="25">
         <v>1</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="25">
+        <v>1</v>
+      </c>
+      <c r="H9" s="23">
+        <v>18624000</v>
+      </c>
+      <c r="I9" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="K9" s="23" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>16</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="23">
+        <v>424519000</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>247</v>
-      </c>
-      <c r="E10" s="25">
-        <v>1</v>
       </c>
       <c r="F10" s="25">
         <v>1</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="25">
+        <v>1</v>
+      </c>
+      <c r="H10" s="23">
+        <v>18624000</v>
+      </c>
+      <c r="I10" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="K10" s="23" t="s">
         <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>17</v>
+      </c>
+      <c r="D11" s="23">
+        <v>1119305005</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="F11" s="25">
+        <v>1</v>
+      </c>
+      <c r="G11" s="25">
+        <v>1</v>
+      </c>
+      <c r="H11" s="23">
+        <v>40733004</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>18</v>
+      </c>
+      <c r="D12" s="23">
+        <v>1119305005</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="F12" s="25">
+        <v>1</v>
+      </c>
+      <c r="G12" s="25">
+        <v>1</v>
+      </c>
+      <c r="H12" s="23">
+        <v>40733004</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>19</v>
+      </c>
+      <c r="D13" s="23">
+        <v>1119305005</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="F13" s="25">
+        <v>1</v>
+      </c>
+      <c r="G13" s="25">
+        <v>1</v>
+      </c>
+      <c r="H13" s="23">
+        <v>40733004</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>20</v>
+      </c>
+      <c r="D14" s="23">
+        <v>1119349007</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="F14" s="25">
+        <v>1</v>
+      </c>
+      <c r="G14" s="25">
+        <v>1</v>
+      </c>
+      <c r="H14" s="23">
+        <v>40733004</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>21</v>
+      </c>
+      <c r="D15" s="23">
+        <v>1119349007</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>390</v>
+      </c>
+      <c r="F15" s="25">
+        <v>1</v>
+      </c>
+      <c r="G15" s="25">
+        <v>1</v>
+      </c>
+      <c r="H15" s="23">
+        <v>40733004</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Form changes and Patient35-38 added
</commit_message>
<xml_diff>
--- a/TestData/TestdataOverview.xlsx
+++ b/TestData/TestdataOverview.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="23715" windowHeight="8265" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="23715" windowHeight="8265" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Movement" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="406">
   <si>
     <t>Impfstoff</t>
   </si>
@@ -1202,6 +1202,45 @@
   </si>
   <si>
     <t>2021-01-08T16:35:00Z</t>
+  </si>
+  <si>
+    <t>00000035</t>
+  </si>
+  <si>
+    <t>2021-01-05T10:30:00Z</t>
+  </si>
+  <si>
+    <t>2021-01-10T11:30:00Z</t>
+  </si>
+  <si>
+    <t>00000036</t>
+  </si>
+  <si>
+    <t>2021-01-04T11:30:00Z</t>
+  </si>
+  <si>
+    <t>2021-01-08T11:30:00Z</t>
+  </si>
+  <si>
+    <t>2021-01-10T10:30:00Z</t>
+  </si>
+  <si>
+    <t>00000037</t>
+  </si>
+  <si>
+    <t>00000038</t>
+  </si>
+  <si>
+    <t>2021-01-03T10:30:00Z</t>
+  </si>
+  <si>
+    <t>2021-01-06T11:30:00Z</t>
+  </si>
+  <si>
+    <t>2021-01-07T11:30:00Z</t>
+  </si>
+  <si>
+    <t>2021-01-09T10:10:00Z</t>
   </si>
 </sst>
 </file>
@@ -1448,8 +1487,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="B5:K73" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="B5:K73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="B5:K80" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="B5:K80"/>
   <tableColumns count="10">
     <tableColumn id="1" name="//"/>
     <tableColumn id="2" name="ehr_id"/>
@@ -1488,8 +1527,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="B5:O55" totalsRowShown="0">
-  <autoFilter ref="B5:O55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="B5:O68" totalsRowShown="0">
+  <autoFilter ref="B5:O68"/>
   <tableColumns count="14">
     <tableColumn id="1" name="//"/>
     <tableColumn id="2" name="ehr_id"/>
@@ -1516,14 +1555,14 @@
   <tableColumns count="10">
     <tableColumn id="1" name="//" dataDxfId="9"/>
     <tableColumn id="2" name="ehr_id" dataDxfId="8"/>
-    <tableColumn id="9" name="code_string" dataDxfId="1"/>
-    <tableColumn id="3" name="Impfstoff" dataDxfId="7"/>
-    <tableColumn id="4" name="Dosierungsreihenfolge" dataDxfId="6"/>
-    <tableColumn id="5" name="Dosiermenge" dataDxfId="5"/>
-    <tableColumn id="10" name="code_string2" dataDxfId="0"/>
-    <tableColumn id="6" name="Impfung gegen" dataDxfId="4"/>
-    <tableColumn id="7" name="Abwesenheit" dataDxfId="3"/>
-    <tableColumn id="8" name="start_time" dataDxfId="2"/>
+    <tableColumn id="9" name="code_string" dataDxfId="7"/>
+    <tableColumn id="3" name="Impfstoff" dataDxfId="6"/>
+    <tableColumn id="4" name="Dosierungsreihenfolge" dataDxfId="5"/>
+    <tableColumn id="5" name="Dosiermenge" dataDxfId="4"/>
+    <tableColumn id="10" name="code_string2" dataDxfId="3"/>
+    <tableColumn id="6" name="Impfung gegen" dataDxfId="2"/>
+    <tableColumn id="7" name="Abwesenheit" dataDxfId="1"/>
+    <tableColumn id="8" name="start_time" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1833,10 +1872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K72"/>
+  <dimension ref="A2:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3822,6 +3861,139 @@
       </c>
       <c r="K72" s="23" t="s">
         <v>358</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>35</v>
+      </c>
+      <c r="D73" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="E73" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F73" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G73" s="23" t="s">
+        <v>394</v>
+      </c>
+      <c r="I73" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="J73" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="K73" s="23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>36</v>
+      </c>
+      <c r="D74" s="26" t="s">
+        <v>353</v>
+      </c>
+      <c r="E74" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F74" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="G74" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="I74" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="J74" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="K74" s="23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>37</v>
+      </c>
+      <c r="D75" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="E75" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F75" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G75" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="I75" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="J75" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="K75" s="23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>38</v>
+      </c>
+      <c r="D76" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="E76" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F76" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G76" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="H76" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="I76" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="J76" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="K76" s="23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>38</v>
+      </c>
+      <c r="D77" s="23" t="s">
+        <v>311</v>
+      </c>
+      <c r="E77" s="26">
+        <v>3700</v>
+      </c>
+      <c r="F77" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G77" s="23" t="s">
+        <v>405</v>
+      </c>
+      <c r="I77" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="J77" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="K77" s="23" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -4787,8 +4959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6859,82 +7031,461 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="M52" s="23"/>
-      <c r="N52" s="23"/>
-      <c r="O52" s="25"/>
+      <c r="B52">
+        <v>35</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="F52" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="G52" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="H52" s="23" t="s">
+        <v>394</v>
+      </c>
+      <c r="I52" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J52" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K52" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="L52" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="M52" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N52" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O52" s="25">
+        <v>30</v>
+      </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="M53" s="23"/>
-      <c r="N53" s="23"/>
-      <c r="O53" s="25"/>
+      <c r="B53">
+        <v>35</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="F53" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="G53" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="H53" s="23" t="s">
+        <v>395</v>
+      </c>
+      <c r="I53" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J53" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K53" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="L53" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="M53" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N53" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O53" s="25">
+        <v>13</v>
+      </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="M54" s="23"/>
-      <c r="N54" s="23"/>
-      <c r="O54" s="25"/>
+      <c r="B54">
+        <v>36</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="F54" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="G54" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="H54" s="23" t="s">
+        <v>397</v>
+      </c>
+      <c r="I54" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J54" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K54" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="L54" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="M54" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N54" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O54" s="25">
+        <v>33</v>
+      </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="M55" s="23"/>
-      <c r="N55" s="23"/>
-      <c r="O55" s="25"/>
+      <c r="B55">
+        <v>36</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="F55" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="G55" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="H55" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="I55" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J55" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K55" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="L55" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="M55" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N55" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O55" s="25">
+        <v>16</v>
+      </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="M56" s="23"/>
-      <c r="N56" s="23"/>
-      <c r="O56" s="25"/>
+      <c r="B56">
+        <v>36</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="F56" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="H56" s="23" t="s">
+        <v>399</v>
+      </c>
+      <c r="I56" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J56" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K56" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="L56" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="M56" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N56" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O56" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="M57" s="23"/>
-      <c r="N57" s="23"/>
-      <c r="O57" s="25"/>
+      <c r="B57">
+        <v>37</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="F57" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="G57" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="H57" s="23" t="s">
+        <v>402</v>
+      </c>
+      <c r="I57" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J57" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K57" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="L57" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="M57" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N57" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O57" s="25">
+        <v>16</v>
+      </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="M58" s="23"/>
-      <c r="N58" s="23"/>
-      <c r="O58" s="25"/>
+      <c r="B58">
+        <v>37</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="F58" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="G58" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>403</v>
+      </c>
+      <c r="I58" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J58" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K58" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="L58" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="M58" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N58" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O58" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="M59" s="23"/>
-      <c r="N59" s="23"/>
-      <c r="O59" s="25"/>
+      <c r="B59">
+        <v>37</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="F59" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="I59" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J59" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K59" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="L59" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="M59" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N59" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O59" s="25">
+        <v>13</v>
+      </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D60" s="27"/>
-      <c r="E60" s="27"/>
-      <c r="M60" s="23"/>
-      <c r="N60" s="23"/>
-      <c r="O60" s="25"/>
+      <c r="B60">
+        <v>38</v>
+      </c>
+      <c r="D60" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="F60" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="G60" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="I60" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J60" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K60" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="L60" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="M60" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N60" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O60" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
-      <c r="M61" s="23"/>
-      <c r="N61" s="23"/>
-      <c r="O61" s="25"/>
+      <c r="B61">
+        <v>38</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="F61" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="H61" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="I61" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J61" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K61" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="L61" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="M61" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N61" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O61" s="25">
+        <v>17</v>
+      </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
+      <c r="B62">
+        <v>38</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E62" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="F62" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="G62" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="H62" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="I62" s="23">
+        <v>119342007</v>
+      </c>
+      <c r="J62" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K62" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="L62" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="M62" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N62" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O62" s="25">
+        <v>33</v>
+      </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D63" s="27"/>
       <c r="E63" s="27"/>
+      <c r="M63" s="23"/>
+      <c r="N63" s="23"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D64" s="27"/>
@@ -7401,7 +7952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -7818,10 +8369,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I39"/>
+  <dimension ref="A2:I43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8550,6 +9101,62 @@
         <v>329</v>
       </c>
     </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>35</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="G40" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="I40" s="26" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>36</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>37</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="G42" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>38</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
symp and vacc tests fixed
</commit_message>
<xml_diff>
--- a/TestData/TestdataOverview.xlsx
+++ b/TestData/TestdataOverview.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="23715" windowHeight="8265" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="23715" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Movement" sheetId="1" r:id="rId1"/>
@@ -4009,8 +4009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4217,7 +4217,7 @@
         <v>118</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>95</v>
@@ -4959,7 +4959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed some Tests, To-DO: EpiCurve, Network, RKIStatistikTests
</commit_message>
<xml_diff>
--- a/TestData/TestdataOverview.xlsx
+++ b/TestData/TestdataOverview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\B-FAST\TestDataNEW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\B-FAST\GITHub_SmICS\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="550">
   <si>
     <t>Impfstoff</t>
   </si>
@@ -1112,9 +1112,6 @@
   </si>
   <si>
     <t>2020-12-01T09:13:09Z</t>
-  </si>
-  <si>
-    <t>2020-11-26T12:13:00Z</t>
   </si>
   <si>
     <t>2020-02-05T12:13:00Z</t>
@@ -2313,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2441,7 +2438,7 @@
         <v>355</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I6" s="22" t="s">
         <v>104</v>
@@ -2467,10 +2464,10 @@
         <v>103</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I7" s="22" t="s">
         <v>104</v>
@@ -2499,7 +2496,7 @@
         <v>336</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I8" s="22" t="s">
         <v>124</v>
@@ -2528,7 +2525,7 @@
         <v>335</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I9" s="22" t="s">
         <v>124</v>
@@ -2554,10 +2551,10 @@
         <v>136</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I10" s="22" t="s">
         <v>137</v>
@@ -2583,10 +2580,10 @@
         <v>136</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I11" s="22" t="s">
         <v>138</v>
@@ -2612,10 +2609,10 @@
         <v>136</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I12" s="22" t="s">
         <v>137</v>
@@ -2641,10 +2638,10 @@
         <v>136</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I13" s="22" t="s">
         <v>137</v>
@@ -2670,10 +2667,10 @@
         <v>136</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I14" s="22" t="s">
         <v>142</v>
@@ -2699,10 +2696,10 @@
         <v>136</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I15" s="22" t="s">
         <v>142</v>
@@ -2728,10 +2725,10 @@
         <v>139</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I16" s="22" t="s">
         <v>104</v>
@@ -2757,10 +2754,10 @@
         <v>140</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I17" s="22" t="s">
         <v>137</v>
@@ -2786,10 +2783,10 @@
         <v>139</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I18" s="22" t="s">
         <v>104</v>
@@ -2815,10 +2812,10 @@
         <v>139</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I19" s="22" t="s">
         <v>124</v>
@@ -2844,10 +2841,10 @@
         <v>139</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I20" s="22" t="s">
         <v>104</v>
@@ -2873,10 +2870,10 @@
         <v>139</v>
       </c>
       <c r="G21" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="H21" s="22" t="s">
         <v>408</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>409</v>
       </c>
       <c r="I21" s="22" t="s">
         <v>104</v>
@@ -2902,10 +2899,10 @@
         <v>141</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I22" s="22" t="s">
         <v>104</v>
@@ -2931,10 +2928,10 @@
         <v>136</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I23" s="22" t="s">
         <v>137</v>
@@ -2960,10 +2957,10 @@
         <v>139</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I24" s="22" t="s">
         <v>104</v>
@@ -2989,10 +2986,10 @@
         <v>139</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I25" s="22" t="s">
         <v>104</v>
@@ -3018,10 +3015,10 @@
         <v>141</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I26" s="22" t="s">
         <v>104</v>
@@ -3047,10 +3044,10 @@
         <v>141</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I27" s="22" t="s">
         <v>104</v>
@@ -3076,10 +3073,10 @@
         <v>136</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I28" s="22" t="s">
         <v>104</v>
@@ -3105,10 +3102,10 @@
         <v>141</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I29" s="22" t="s">
         <v>104</v>
@@ -3134,10 +3131,10 @@
         <v>141</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I30" s="22" t="s">
         <v>104</v>
@@ -3163,10 +3160,10 @@
         <v>136</v>
       </c>
       <c r="G31" s="22" t="s">
+        <v>419</v>
+      </c>
+      <c r="H31" s="22" t="s">
         <v>420</v>
-      </c>
-      <c r="H31" s="22" t="s">
-        <v>421</v>
       </c>
       <c r="I31" s="22" t="s">
         <v>104</v>
@@ -3192,10 +3189,10 @@
         <v>141</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I32" s="22" t="s">
         <v>104</v>
@@ -3221,10 +3218,10 @@
         <v>254</v>
       </c>
       <c r="G33" s="22" t="s">
+        <v>423</v>
+      </c>
+      <c r="H33" s="22" t="s">
         <v>424</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>425</v>
       </c>
       <c r="I33" s="22" t="s">
         <v>104</v>
@@ -3253,7 +3250,7 @@
         <v>141</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I34" s="22" t="s">
         <v>104</v>
@@ -3282,7 +3279,7 @@
         <v>141</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I35" s="22" t="s">
         <v>104</v>
@@ -3308,7 +3305,7 @@
         <v>141</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I36" s="22" t="s">
         <v>104</v>
@@ -3337,7 +3334,7 @@
         <v>141</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I37" s="22" t="s">
         <v>104</v>
@@ -3366,7 +3363,7 @@
         <v>141</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I38" s="22" t="s">
         <v>104</v>
@@ -3395,7 +3392,7 @@
         <v>141</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I39" s="22" t="s">
         <v>104</v>
@@ -3421,10 +3418,10 @@
         <v>136</v>
       </c>
       <c r="G40" s="22" t="s">
+        <v>431</v>
+      </c>
+      <c r="H40" s="22" t="s">
         <v>432</v>
-      </c>
-      <c r="H40" s="22" t="s">
-        <v>433</v>
       </c>
       <c r="I40" s="22" t="s">
         <v>104</v>
@@ -3450,10 +3447,10 @@
         <v>141</v>
       </c>
       <c r="G41" s="22" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H41" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I41" s="22" t="s">
         <v>104</v>
@@ -3479,7 +3476,7 @@
         <v>141</v>
       </c>
       <c r="G42" s="22" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I42" s="22" t="s">
         <v>104</v>
@@ -3505,7 +3502,7 @@
         <v>141</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I43" s="22" t="s">
         <v>104</v>
@@ -3531,7 +3528,7 @@
         <v>141</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I44" s="22" t="s">
         <v>104</v>
@@ -3557,10 +3554,10 @@
         <v>136</v>
       </c>
       <c r="G45" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="H45" s="22" t="s">
         <v>438</v>
-      </c>
-      <c r="H45" s="22" t="s">
-        <v>439</v>
       </c>
       <c r="I45" s="22" t="s">
         <v>104</v>
@@ -3586,7 +3583,7 @@
         <v>141</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I46" s="22" t="s">
         <v>104</v>
@@ -3612,10 +3609,10 @@
         <v>141</v>
       </c>
       <c r="G47" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="H47" s="22" t="s">
         <v>441</v>
-      </c>
-      <c r="H47" s="22" t="s">
-        <v>442</v>
       </c>
       <c r="I47" s="22" t="s">
         <v>104</v>
@@ -3641,7 +3638,7 @@
         <v>141</v>
       </c>
       <c r="G48" s="22" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I48" s="22" t="s">
         <v>104</v>
@@ -3667,10 +3664,10 @@
         <v>136</v>
       </c>
       <c r="G49" s="22" t="s">
+        <v>443</v>
+      </c>
+      <c r="H49" s="22" t="s">
         <v>444</v>
-      </c>
-      <c r="H49" s="22" t="s">
-        <v>445</v>
       </c>
       <c r="I49" s="22" t="s">
         <v>104</v>
@@ -3696,10 +3693,10 @@
         <v>141</v>
       </c>
       <c r="G50" s="22" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I50" s="22" t="s">
         <v>104</v>
@@ -3725,10 +3722,10 @@
         <v>141</v>
       </c>
       <c r="G51" s="22" t="s">
+        <v>447</v>
+      </c>
+      <c r="H51" s="22" t="s">
         <v>448</v>
-      </c>
-      <c r="H51" s="22" t="s">
-        <v>449</v>
       </c>
       <c r="I51" s="22" t="s">
         <v>104</v>
@@ -3754,7 +3751,7 @@
         <v>254</v>
       </c>
       <c r="G52" s="22" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I52" s="22" t="s">
         <v>104</v>
@@ -3780,7 +3777,7 @@
         <v>141</v>
       </c>
       <c r="G53" s="22" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I53" s="22" t="s">
         <v>104</v>
@@ -3806,10 +3803,10 @@
         <v>141</v>
       </c>
       <c r="G54" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="H54" s="22" t="s">
         <v>452</v>
-      </c>
-      <c r="H54" s="22" t="s">
-        <v>453</v>
       </c>
       <c r="I54" s="22" t="s">
         <v>104</v>
@@ -3835,7 +3832,7 @@
         <v>254</v>
       </c>
       <c r="G55" s="22" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I55" s="22" t="s">
         <v>104</v>
@@ -3861,10 +3858,10 @@
         <v>303</v>
       </c>
       <c r="G56" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="H56" s="22" t="s">
         <v>455</v>
-      </c>
-      <c r="H56" s="22" t="s">
-        <v>456</v>
       </c>
       <c r="I56" s="22" t="s">
         <v>301</v>
@@ -3890,10 +3887,10 @@
         <v>140</v>
       </c>
       <c r="G57" s="22" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H57" s="22" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I57" s="22" t="s">
         <v>301</v>
@@ -3919,10 +3916,10 @@
         <v>141</v>
       </c>
       <c r="G58" s="22" t="s">
+        <v>458</v>
+      </c>
+      <c r="H58" s="22" t="s">
         <v>459</v>
-      </c>
-      <c r="H58" s="22" t="s">
-        <v>460</v>
       </c>
       <c r="I58" s="22" t="s">
         <v>301</v>
@@ -3948,10 +3945,10 @@
         <v>141</v>
       </c>
       <c r="G59" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="H59" s="22" t="s">
         <v>461</v>
-      </c>
-      <c r="H59" s="22" t="s">
-        <v>462</v>
       </c>
       <c r="I59" s="22" t="s">
         <v>301</v>
@@ -3977,10 +3974,10 @@
         <v>308</v>
       </c>
       <c r="G60" s="22" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H60" s="22" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I60" s="22" t="s">
         <v>301</v>
@@ -4006,10 +4003,10 @@
         <v>310</v>
       </c>
       <c r="G61" s="22" t="s">
+        <v>464</v>
+      </c>
+      <c r="H61" s="22" t="s">
         <v>465</v>
-      </c>
-      <c r="H61" s="22" t="s">
-        <v>466</v>
       </c>
       <c r="I61" s="22" t="s">
         <v>301</v>
@@ -4035,10 +4032,10 @@
         <v>141</v>
       </c>
       <c r="G62" s="22" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H62" s="22" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I62" s="22" t="s">
         <v>301</v>
@@ -4064,10 +4061,10 @@
         <v>312</v>
       </c>
       <c r="G63" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="H63" s="22" t="s">
         <v>469</v>
-      </c>
-      <c r="H63" s="22" t="s">
-        <v>470</v>
       </c>
       <c r="I63" s="22" t="s">
         <v>301</v>
@@ -4093,10 +4090,10 @@
         <v>314</v>
       </c>
       <c r="G64" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="H64" s="22" t="s">
         <v>471</v>
-      </c>
-      <c r="H64" s="22" t="s">
-        <v>472</v>
       </c>
       <c r="I64" s="22" t="s">
         <v>301</v>
@@ -4122,10 +4119,10 @@
         <v>312</v>
       </c>
       <c r="G65" s="22" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H65" s="22" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I65" s="22" t="s">
         <v>301</v>
@@ -4151,10 +4148,10 @@
         <v>141</v>
       </c>
       <c r="G66" s="22" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H66" s="22" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I66" s="22" t="s">
         <v>301</v>
@@ -4180,10 +4177,10 @@
         <v>141</v>
       </c>
       <c r="G67" s="22" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H67" s="22" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I67" s="22" t="s">
         <v>301</v>
@@ -4209,10 +4206,10 @@
         <v>141</v>
       </c>
       <c r="G68" s="22" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H68" s="22" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I68" s="22" t="s">
         <v>301</v>
@@ -4238,10 +4235,10 @@
         <v>141</v>
       </c>
       <c r="G69" s="22" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H69" s="22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I69" s="22" t="s">
         <v>301</v>
@@ -4267,10 +4264,10 @@
         <v>141</v>
       </c>
       <c r="G70" s="22" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H70" s="22" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I70" s="22" t="s">
         <v>301</v>
@@ -4296,10 +4293,10 @@
         <v>314</v>
       </c>
       <c r="G71" s="22" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H71" s="22" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I71" s="22" t="s">
         <v>301</v>
@@ -4325,10 +4322,10 @@
         <v>310</v>
       </c>
       <c r="G72" s="22" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H72" s="22" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I72" s="22" t="s">
         <v>301</v>
@@ -4354,7 +4351,7 @@
         <v>141</v>
       </c>
       <c r="G73" s="22" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I73" s="22" t="s">
         <v>104</v>
@@ -4380,7 +4377,7 @@
         <v>136</v>
       </c>
       <c r="G74" s="22" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I74" s="22" t="s">
         <v>104</v>
@@ -4406,7 +4403,7 @@
         <v>141</v>
       </c>
       <c r="G75" s="22" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I75" s="22" t="s">
         <v>104</v>
@@ -4432,7 +4429,7 @@
         <v>141</v>
       </c>
       <c r="G76" s="22" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H76" s="22" t="s">
         <v>333</v>
@@ -4461,7 +4458,7 @@
         <v>141</v>
       </c>
       <c r="G77" s="22" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I77" s="22" t="s">
         <v>124</v>
@@ -4491,13 +4488,13 @@
         <v>266</v>
       </c>
       <c r="H78" s="22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I78" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J78" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K78" s="22" t="s">
         <v>102</v>
@@ -4520,13 +4517,13 @@
         <v>270</v>
       </c>
       <c r="H79" s="22" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I79" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J79" s="25" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K79" s="22" t="s">
         <v>102</v>
@@ -4546,16 +4543,16 @@
         <v>141</v>
       </c>
       <c r="G80" s="22" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H80" s="22" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I80" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J80" s="25" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K80" s="22" t="s">
         <v>102</v>
@@ -4575,16 +4572,16 @@
         <v>141</v>
       </c>
       <c r="G81" s="22" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H81" s="22" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I81" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J81" s="25" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="K81" s="22" t="s">
         <v>102</v>
@@ -4604,16 +4601,16 @@
         <v>141</v>
       </c>
       <c r="G82" s="22" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H82" s="22" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I82" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J82" s="25" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K82" s="22" t="s">
         <v>102</v>
@@ -4633,16 +4630,16 @@
         <v>141</v>
       </c>
       <c r="G83" s="22" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H83" s="22" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I83" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J83" s="25" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K83" s="22" t="s">
         <v>102</v>
@@ -4662,16 +4659,16 @@
         <v>141</v>
       </c>
       <c r="G84" s="22" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H84" s="22" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I84" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J84" s="25" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K84" s="22" t="s">
         <v>102</v>
@@ -4691,16 +4688,16 @@
         <v>141</v>
       </c>
       <c r="G85" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H85" s="22" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I85" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J85" s="25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="K85" s="22" t="s">
         <v>102</v>
@@ -4720,16 +4717,16 @@
         <v>141</v>
       </c>
       <c r="G86" s="22" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H86" s="22" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I86" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J86" s="25" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K86" s="22" t="s">
         <v>102</v>
@@ -4749,16 +4746,16 @@
         <v>141</v>
       </c>
       <c r="G87" s="22" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H87" s="22" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I87" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J87" s="25" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K87" s="22" t="s">
         <v>102</v>
@@ -4778,16 +4775,16 @@
         <v>141</v>
       </c>
       <c r="G88" s="22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H88" s="22" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I88" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J88" s="25" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K88" s="22" t="s">
         <v>102</v>
@@ -4807,16 +4804,16 @@
         <v>141</v>
       </c>
       <c r="G89" s="22" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H89" s="22" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I89" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J89" s="25" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K89" s="22" t="s">
         <v>102</v>
@@ -4836,13 +4833,13 @@
         <v>141</v>
       </c>
       <c r="G90" s="22" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I90" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J90" s="25" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K90" s="22" t="s">
         <v>102</v>
@@ -4862,13 +4859,13 @@
         <v>141</v>
       </c>
       <c r="G91" s="22" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I91" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J91" s="25" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="K91" s="22" t="s">
         <v>102</v>
@@ -4888,13 +4885,13 @@
         <v>141</v>
       </c>
       <c r="G92" s="22" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I92" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J92" s="25" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K92" s="22" t="s">
         <v>102</v>
@@ -4914,13 +4911,13 @@
         <v>141</v>
       </c>
       <c r="G93" s="22" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I93" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J93" s="25" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K93" s="22" t="s">
         <v>102</v>
@@ -4940,13 +4937,13 @@
         <v>141</v>
       </c>
       <c r="G94" s="22" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I94" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J94" s="25" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K94" s="22" t="s">
         <v>102</v>
@@ -4966,13 +4963,13 @@
         <v>141</v>
       </c>
       <c r="G95" s="22" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I95" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J95" s="25" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K95" s="22" t="s">
         <v>102</v>
@@ -4992,13 +4989,13 @@
         <v>141</v>
       </c>
       <c r="G96" s="22" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I96" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J96" s="25" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K96" s="22" t="s">
         <v>102</v>
@@ -5018,13 +5015,13 @@
         <v>141</v>
       </c>
       <c r="G97" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I97" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J97" s="25" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K97" s="22" t="s">
         <v>102</v>
@@ -5044,13 +5041,13 @@
         <v>141</v>
       </c>
       <c r="G98" s="22" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I98" s="22" t="s">
         <v>104</v>
       </c>
       <c r="J98" s="25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K98" s="22" t="s">
         <v>102</v>
@@ -6019,7 +6016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O172"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -6233,7 +6230,7 @@
         <v>293</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I7" s="22">
         <v>119342007</v>
@@ -6245,7 +6242,7 @@
         <v>160</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>146</v>
@@ -9180,7 +9177,7 @@
         <v>144</v>
       </c>
       <c r="E78" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F78" s="25" t="s">
         <v>232</v>
@@ -9189,7 +9186,7 @@
         <v>266</v>
       </c>
       <c r="H78" s="22" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I78" s="22">
         <v>119342007</v>
@@ -9222,7 +9219,7 @@
         <v>144</v>
       </c>
       <c r="E79" s="25" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F79" s="25" t="s">
         <v>232</v>
@@ -9231,7 +9228,7 @@
         <v>270</v>
       </c>
       <c r="H79" s="22" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I79" s="22">
         <v>119342007</v>
@@ -9263,16 +9260,16 @@
         <v>144</v>
       </c>
       <c r="E80" s="25" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F80" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G80" s="22" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H80" s="22" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I80" s="22">
         <v>119342007</v>
@@ -9284,7 +9281,7 @@
         <v>160</v>
       </c>
       <c r="L80" s="22" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="M80" s="22" t="s">
         <v>146</v>
@@ -9304,16 +9301,16 @@
         <v>144</v>
       </c>
       <c r="E81" s="25" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F81" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G81" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="H81" s="22" t="s">
         <v>513</v>
-      </c>
-      <c r="H81" s="22" t="s">
-        <v>514</v>
       </c>
       <c r="I81" s="22">
         <v>119342007</v>
@@ -9325,7 +9322,7 @@
         <v>160</v>
       </c>
       <c r="L81" s="22" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="M81" s="22" t="s">
         <v>146</v>
@@ -9345,16 +9342,16 @@
         <v>144</v>
       </c>
       <c r="E82" s="25" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F82" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G82" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="H82" s="22" t="s">
         <v>514</v>
-      </c>
-      <c r="H82" s="22" t="s">
-        <v>515</v>
       </c>
       <c r="I82" s="22">
         <v>119342007</v>
@@ -9366,7 +9363,7 @@
         <v>160</v>
       </c>
       <c r="L82" s="22" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M82" s="22" t="s">
         <v>146</v>
@@ -9386,16 +9383,16 @@
         <v>144</v>
       </c>
       <c r="E83" s="25" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F83" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G83" s="22" t="s">
+        <v>514</v>
+      </c>
+      <c r="H83" s="22" t="s">
         <v>515</v>
-      </c>
-      <c r="H83" s="22" t="s">
-        <v>516</v>
       </c>
       <c r="I83" s="22">
         <v>119342007</v>
@@ -9407,7 +9404,7 @@
         <v>160</v>
       </c>
       <c r="L83" s="22" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="M83" s="22" t="s">
         <v>146</v>
@@ -9427,16 +9424,16 @@
         <v>144</v>
       </c>
       <c r="E84" s="25" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F84" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G84" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="H84" s="22" t="s">
         <v>516</v>
-      </c>
-      <c r="H84" s="22" t="s">
-        <v>517</v>
       </c>
       <c r="I84" s="22">
         <v>119342007</v>
@@ -9448,7 +9445,7 @@
         <v>160</v>
       </c>
       <c r="L84" s="22" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="M84" s="22" t="s">
         <v>146</v>
@@ -9468,16 +9465,16 @@
         <v>144</v>
       </c>
       <c r="E85" s="25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F85" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G85" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H85" s="22" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I85" s="22">
         <v>119342007</v>
@@ -9489,7 +9486,7 @@
         <v>160</v>
       </c>
       <c r="L85" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="M85" s="22" t="s">
         <v>146</v>
@@ -9509,16 +9506,16 @@
         <v>144</v>
       </c>
       <c r="E86" s="25" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F86" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G86" s="22" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H86" s="22" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I86" s="22">
         <v>119342007</v>
@@ -9530,7 +9527,7 @@
         <v>160</v>
       </c>
       <c r="L86" s="22" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="M86" s="22" t="s">
         <v>146</v>
@@ -9550,16 +9547,16 @@
         <v>144</v>
       </c>
       <c r="E87" s="25" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F87" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G87" s="22" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H87" s="22" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I87" s="22">
         <v>119342007</v>
@@ -9571,7 +9568,7 @@
         <v>160</v>
       </c>
       <c r="L87" s="22" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="M87" s="22" t="s">
         <v>146</v>
@@ -9591,16 +9588,16 @@
         <v>144</v>
       </c>
       <c r="E88" s="25" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F88" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G88" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="H88" s="22" t="s">
         <v>520</v>
-      </c>
-      <c r="H88" s="22" t="s">
-        <v>521</v>
       </c>
       <c r="I88" s="22">
         <v>119342007</v>
@@ -9612,7 +9609,7 @@
         <v>160</v>
       </c>
       <c r="L88" s="22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="M88" s="22" t="s">
         <v>146</v>
@@ -9632,16 +9629,16 @@
         <v>144</v>
       </c>
       <c r="E89" s="25" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F89" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G89" s="22" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H89" s="22" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I89" s="22">
         <v>119342007</v>
@@ -9653,7 +9650,7 @@
         <v>160</v>
       </c>
       <c r="L89" s="22" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="M89" s="22" t="s">
         <v>146</v>
@@ -9673,16 +9670,16 @@
         <v>144</v>
       </c>
       <c r="E90" s="25" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F90" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G90" s="22" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H90" s="22" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I90" s="22">
         <v>119342007</v>
@@ -9694,7 +9691,7 @@
         <v>160</v>
       </c>
       <c r="L90" s="22" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="M90" s="22" t="s">
         <v>146</v>
@@ -9714,16 +9711,16 @@
         <v>144</v>
       </c>
       <c r="E91" s="25" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F91" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G91" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="H91" s="22" t="s">
         <v>523</v>
-      </c>
-      <c r="H91" s="22" t="s">
-        <v>524</v>
       </c>
       <c r="I91" s="22">
         <v>119342007</v>
@@ -9735,7 +9732,7 @@
         <v>160</v>
       </c>
       <c r="L91" s="22" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="M91" s="22" t="s">
         <v>146</v>
@@ -9755,16 +9752,16 @@
         <v>144</v>
       </c>
       <c r="E92" s="25" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F92" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G92" s="22" t="s">
+        <v>523</v>
+      </c>
+      <c r="H92" s="22" t="s">
         <v>524</v>
-      </c>
-      <c r="H92" s="22" t="s">
-        <v>525</v>
       </c>
       <c r="I92" s="22">
         <v>119342007</v>
@@ -9776,7 +9773,7 @@
         <v>160</v>
       </c>
       <c r="L92" s="22" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="M92" s="22" t="s">
         <v>146</v>
@@ -9796,16 +9793,16 @@
         <v>144</v>
       </c>
       <c r="E93" s="25" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F93" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G93" s="22" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H93" s="22" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I93" s="22">
         <v>119342007</v>
@@ -9817,7 +9814,7 @@
         <v>160</v>
       </c>
       <c r="L93" s="22" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="M93" s="22" t="s">
         <v>146</v>
@@ -9837,16 +9834,16 @@
         <v>144</v>
       </c>
       <c r="E94" s="25" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F94" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G94" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="H94" s="22" t="s">
         <v>526</v>
-      </c>
-      <c r="H94" s="22" t="s">
-        <v>527</v>
       </c>
       <c r="I94" s="22">
         <v>119342007</v>
@@ -9858,7 +9855,7 @@
         <v>160</v>
       </c>
       <c r="L94" s="22" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="M94" s="22" t="s">
         <v>146</v>
@@ -9878,16 +9875,16 @@
         <v>144</v>
       </c>
       <c r="E95" s="25" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F95" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G95" s="22" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H95" s="22" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I95" s="22">
         <v>119342007</v>
@@ -9899,7 +9896,7 @@
         <v>160</v>
       </c>
       <c r="L95" s="22" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="M95" s="22" t="s">
         <v>146</v>
@@ -9919,16 +9916,16 @@
         <v>144</v>
       </c>
       <c r="E96" s="25" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F96" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G96" s="22" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H96" s="22" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I96" s="22">
         <v>119342007</v>
@@ -9940,7 +9937,7 @@
         <v>160</v>
       </c>
       <c r="L96" s="22" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="M96" s="22" t="s">
         <v>146</v>
@@ -9960,16 +9957,16 @@
         <v>144</v>
       </c>
       <c r="E97" s="25" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F97" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G97" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H97" s="22" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I97" s="22">
         <v>119342007</v>
@@ -9981,7 +9978,7 @@
         <v>160</v>
       </c>
       <c r="L97" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M97" s="22" t="s">
         <v>146</v>
@@ -10001,16 +9998,16 @@
         <v>144</v>
       </c>
       <c r="E98" s="25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F98" s="25" t="s">
         <v>232</v>
       </c>
       <c r="G98" s="22" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H98" s="22" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I98" s="22">
         <v>119342007</v>
@@ -10022,7 +10019,7 @@
         <v>160</v>
       </c>
       <c r="L98" s="22" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="M98" s="22" t="s">
         <v>146</v>
@@ -10781,8 +10778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J64"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44:H55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10866,7 +10863,7 @@
         <v>355</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I6" s="25" t="s">
         <v>277</v>
@@ -10886,10 +10883,10 @@
         <v>114</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I7" s="25" t="s">
         <v>278</v>
@@ -10912,7 +10909,7 @@
         <v>336</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I8" s="25" t="s">
         <v>279</v>
@@ -10935,7 +10932,7 @@
         <v>335</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I9" s="25" t="s">
         <v>280</v>
@@ -10955,10 +10952,10 @@
         <v>114</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I10" s="25" t="s">
         <v>281</v>
@@ -10978,10 +10975,10 @@
         <v>114</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I11" s="25" t="s">
         <v>282</v>
@@ -11001,10 +10998,10 @@
         <v>114</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I12" s="25" t="s">
         <v>283</v>
@@ -11024,10 +11021,10 @@
         <v>114</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I13" s="25" t="s">
         <v>284</v>
@@ -11047,10 +11044,10 @@
         <v>114</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I14" s="25" t="s">
         <v>285</v>
@@ -11070,10 +11067,10 @@
         <v>114</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I15" s="25" t="s">
         <v>290</v>
@@ -11096,7 +11093,7 @@
         <v>349</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I16" s="25" t="s">
         <v>286</v>
@@ -11116,10 +11113,10 @@
         <v>114</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I17" s="25" t="s">
         <v>287</v>
@@ -11142,7 +11139,7 @@
         <v>351</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I18" s="25" t="s">
         <v>288</v>
@@ -11162,10 +11159,10 @@
         <v>114</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I19" s="25" t="s">
         <v>289</v>
@@ -11185,10 +11182,10 @@
         <v>114</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I20" s="25" t="s">
         <v>291</v>
@@ -11208,10 +11205,10 @@
         <v>114</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I21" s="25" t="s">
         <v>292</v>
@@ -11231,10 +11228,10 @@
         <v>114</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I22" s="25" t="s">
         <v>229</v>
@@ -11254,10 +11251,10 @@
         <v>114</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I23" s="25" t="s">
         <v>241</v>
@@ -11277,10 +11274,10 @@
         <v>114</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I24" s="25" t="s">
         <v>240</v>
@@ -11300,10 +11297,10 @@
         <v>114</v>
       </c>
       <c r="G25" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="H25" s="22" t="s">
         <v>380</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>381</v>
       </c>
       <c r="I25" s="25" t="s">
         <v>250</v>
@@ -11319,7 +11316,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I26" s="25" t="s">
         <v>253</v>
@@ -11335,7 +11332,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I27" s="25" t="s">
         <v>257</v>
@@ -11351,7 +11348,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I28" s="25" t="s">
         <v>258</v>
@@ -11365,7 +11362,7 @@
         <v>112</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I29" s="25" t="s">
         <v>259</v>
@@ -11379,7 +11376,7 @@
         <v>112</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I30" s="25" t="s">
         <v>262</v>
@@ -11393,7 +11390,7 @@
         <v>112</v>
       </c>
       <c r="G31" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I31" s="25" t="s">
         <v>263</v>
@@ -11407,7 +11404,7 @@
         <v>112</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I32" s="25" t="s">
         <v>264</v>
@@ -11421,7 +11418,7 @@
         <v>112</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I33" s="25" t="s">
         <v>268</v>
@@ -11435,7 +11432,7 @@
         <v>112</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I34" s="25" t="s">
         <v>269</v>
@@ -11449,7 +11446,7 @@
         <v>112</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I35" s="25" t="s">
         <v>272</v>
@@ -11463,7 +11460,7 @@
         <v>112</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I36" s="25" t="s">
         <v>273</v>
@@ -11477,7 +11474,7 @@
         <v>112</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I37" s="25" t="s">
         <v>274</v>
@@ -11491,7 +11488,7 @@
         <v>112</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I38" s="25" t="s">
         <v>275</v>
@@ -11505,7 +11502,7 @@
         <v>112</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I39" s="25" t="s">
         <v>276</v>
@@ -11584,10 +11581,10 @@
         <v>266</v>
       </c>
       <c r="H44" s="22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I44" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J44" s="29"/>
     </row>
@@ -11608,10 +11605,10 @@
         <v>270</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I45" s="25" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
@@ -11628,13 +11625,13 @@
         <v>114</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H46" s="22" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I46" s="25" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
@@ -11651,13 +11648,13 @@
         <v>114</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H47" s="22" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I47" s="25" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
@@ -11674,13 +11671,13 @@
         <v>114</v>
       </c>
       <c r="G48" s="22" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H48" s="22" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I48" s="25" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
@@ -11697,13 +11694,13 @@
         <v>114</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H49" s="22" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I49" s="25" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
@@ -11720,13 +11717,13 @@
         <v>114</v>
       </c>
       <c r="G50" s="22" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I50" s="25" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
@@ -11743,13 +11740,13 @@
         <v>114</v>
       </c>
       <c r="G51" s="22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I51" s="25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
@@ -11766,13 +11763,13 @@
         <v>114</v>
       </c>
       <c r="G52" s="22" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H52" s="22" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I52" s="25" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
@@ -11789,13 +11786,13 @@
         <v>114</v>
       </c>
       <c r="G53" s="22" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H53" s="22" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I53" s="25" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
@@ -11812,13 +11809,13 @@
         <v>114</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H54" s="22" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I54" s="25" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
@@ -11835,13 +11832,13 @@
         <v>114</v>
       </c>
       <c r="G55" s="22" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H55" s="22" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I55" s="25" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
@@ -11852,10 +11849,10 @@
         <v>112</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I56" s="25" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
@@ -11866,10 +11863,10 @@
         <v>112</v>
       </c>
       <c r="G57" s="22" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I57" s="25" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
@@ -11880,10 +11877,10 @@
         <v>112</v>
       </c>
       <c r="G58" s="22" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I58" s="25" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
@@ -11894,10 +11891,10 @@
         <v>112</v>
       </c>
       <c r="G59" s="22" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I59" s="25" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
@@ -11908,10 +11905,10 @@
         <v>112</v>
       </c>
       <c r="G60" s="22" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I60" s="25" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
@@ -11922,10 +11919,10 @@
         <v>112</v>
       </c>
       <c r="G61" s="22" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I61" s="25" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
@@ -11936,10 +11933,10 @@
         <v>112</v>
       </c>
       <c r="G62" s="22" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I62" s="25" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
@@ -11950,10 +11947,10 @@
         <v>112</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I63" s="25" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
@@ -11964,10 +11961,10 @@
         <v>112</v>
       </c>
       <c r="G64" s="22" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I64" s="25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>